<commit_message>
Refactor: split UI into modules + add jump-rope metronome
</commit_message>
<xml_diff>
--- a/assets/trainings_list/trainings_list.xlsx
+++ b/assets/trainings_list/trainings_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fa_tra_app\assets\trainings_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFE938D-B844-4EFE-B123-B83AE13CA07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423B6638-77E0-46AD-8D67-5B257E31838A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{94FEC04D-926D-4059-8F31-F3CBE90CDB79}"/>
   </bookViews>
@@ -710,7 +710,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>